<commit_message>
added updated flow diagrams of program functions
</commit_message>
<xml_diff>
--- a/mosfet_pcb_to_arduino_to_code_translation_table.xlsx
+++ b/mosfet_pcb_to_arduino_to_code_translation_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keegan\Documents\GitHub\Capstone_Solar_Cart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA4441CF-A0B5-4396-8B76-10506A0560FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1592C042-1545-41ED-903B-CA0B18CC8344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="1044" windowWidth="30936" windowHeight="17040" xr2:uid="{986B7D76-C553-450F-9A6B-AC96F219F680}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{986B7D76-C553-450F-9A6B-AC96F219F680}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -407,7 +407,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2B5C1A07-8A84-45CA-BD4E-F6293ABBC805}" name="Table24" displayName="Table24" ref="B5:G26" totalsRowShown="0">
   <autoFilter ref="B5:G26" xr:uid="{2B5C1A07-8A84-45CA-BD4E-F6293ABBC805}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B6:G26">
-    <sortCondition ref="G5:G26"/>
+    <sortCondition ref="C5:C26"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{2D6726CC-32F4-43AE-9571-0296FC7FEBB3}" name="FET ID"/>
@@ -720,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F24A7B2-DB7E-428D-9891-696EDAF3C373}">
   <dimension ref="B5:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,22 +758,22 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6">
-        <v>11</v>
+        <v>46</v>
+      </c>
+      <c r="G6" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
@@ -798,382 +798,382 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E8" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G8">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>81</v>
+        <v>15</v>
       </c>
       <c r="E9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9">
-        <v>14</v>
+        <v>48</v>
+      </c>
+      <c r="G9" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E10" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G10">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E11" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G11">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>65</v>
+        <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>86</v>
+        <v>11</v>
       </c>
       <c r="E12" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>66</v>
-      </c>
-      <c r="G12">
-        <v>17</v>
+        <v>54</v>
+      </c>
+      <c r="G12" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>85</v>
+        <v>16</v>
       </c>
       <c r="E13" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F13" t="s">
-        <v>63</v>
-      </c>
-      <c r="G13">
-        <v>18</v>
+        <v>55</v>
+      </c>
+      <c r="G13" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E14" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F14" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="G14">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E15" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F15" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="G15">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
+        <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>89</v>
+        <v>12</v>
       </c>
       <c r="E16" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>76</v>
-      </c>
-      <c r="G16">
-        <v>21</v>
+        <v>62</v>
+      </c>
+      <c r="G16" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D17" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="E17" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F17" t="s">
-        <v>46</v>
-      </c>
-      <c r="G17" t="s">
-        <v>90</v>
+        <v>63</v>
+      </c>
+      <c r="G17">
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E18" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F18" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G18" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>1</v>
+        <v>65</v>
       </c>
       <c r="D19" t="s">
-        <v>15</v>
+        <v>86</v>
       </c>
       <c r="E19" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F19" t="s">
-        <v>48</v>
-      </c>
-      <c r="G19" t="s">
-        <v>91</v>
+        <v>66</v>
+      </c>
+      <c r="G19">
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E20" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F20" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="G20" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D21" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E21" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F21" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="G21" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C22" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="D22" t="s">
-        <v>12</v>
+        <v>87</v>
       </c>
       <c r="E22" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F22" t="s">
-        <v>62</v>
-      </c>
-      <c r="G22" t="s">
-        <v>94</v>
+        <v>70</v>
+      </c>
+      <c r="G22">
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="1">
         <v>5</v>
       </c>
-      <c r="D23" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="1">
-        <v>3</v>
-      </c>
       <c r="F23" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="G23" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C24" t="s">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="D24" t="s">
-        <v>13</v>
+        <v>88</v>
       </c>
       <c r="E24" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F24" t="s">
-        <v>67</v>
-      </c>
-      <c r="G24" t="s">
-        <v>96</v>
+        <v>72</v>
+      </c>
+      <c r="G24">
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C25" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E25" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F25" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="G25" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
       <c r="D26" t="s">
-        <v>14</v>
+        <v>89</v>
       </c>
       <c r="E26" s="1">
         <v>5</v>
       </c>
       <c r="F26" t="s">
-        <v>71</v>
-      </c>
-      <c r="G26" t="s">
-        <v>98</v>
+        <v>76</v>
+      </c>
+      <c r="G26">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>